<commit_message>
dataframe order by values, plot chart
</commit_message>
<xml_diff>
--- a/experiments/experiment_1/notebooks/estrategia1.xlsx
+++ b/experiments/experiment_1/notebooks/estrategia1.xlsx
@@ -76,25 +76,25 @@
     <t>final_accumulated_fmeasure</t>
   </si>
   <si>
+    <t>webofscience</t>
+  </si>
+  <si>
+    <t>springer</t>
+  </si>
+  <si>
+    <t>scopus</t>
+  </si>
+  <si>
     <t>sciencedirect</t>
   </si>
   <si>
-    <t>webofscience</t>
+    <t>ieee</t>
   </si>
   <si>
     <t>elcompendex</t>
   </si>
   <si>
-    <t>springer</t>
-  </si>
-  <si>
     <t>acm</t>
-  </si>
-  <si>
-    <t>ieee</t>
-  </si>
-  <si>
-    <t>scopus</t>
   </si>
   <si>
     <t>s0</t>
@@ -537,13 +537,13 @@
         <v>20</v>
       </c>
       <c r="C2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E2">
-        <v>0.8</v>
+        <v>16.39</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -558,40 +558,40 @@
         <v>28</v>
       </c>
       <c r="J2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="K2">
-        <v>195</v>
+        <v>10</v>
       </c>
       <c r="L2">
         <v>0</v>
       </c>
       <c r="M2">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="N2">
-        <v>195</v>
+        <v>10</v>
       </c>
       <c r="O2">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="P2">
-        <v>0.5</v>
+        <v>50</v>
       </c>
       <c r="Q2">
-        <v>2</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="R2">
-        <v>0.8</v>
+        <v>16.39</v>
       </c>
       <c r="S2">
-        <v>0.005128205128205128</v>
+        <v>0.4</v>
       </c>
       <c r="T2">
-        <v>0.03333333333333333</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="U2">
-        <v>0.008888888888888889</v>
+        <v>0.2</v>
       </c>
     </row>
     <row r="3" spans="1:21">
@@ -602,13 +602,13 @@
         <v>21</v>
       </c>
       <c r="C3">
-        <v>50</v>
+        <v>1.42</v>
       </c>
       <c r="D3">
-        <v>9.800000000000001</v>
+        <v>3.92</v>
       </c>
       <c r="E3">
-        <v>16.4</v>
+        <v>2.08</v>
       </c>
       <c r="F3">
         <v>0</v>
@@ -623,40 +623,40 @@
         <v>28</v>
       </c>
       <c r="J3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="K3">
-        <v>10</v>
+        <v>141</v>
       </c>
       <c r="L3">
         <v>0</v>
       </c>
       <c r="M3">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="N3">
-        <v>10</v>
+        <v>141</v>
       </c>
       <c r="O3">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="P3">
-        <v>50</v>
+        <v>1.42</v>
       </c>
       <c r="Q3">
-        <v>9.800000000000001</v>
+        <v>3.92</v>
       </c>
       <c r="R3">
-        <v>16.4</v>
+        <v>2.08</v>
       </c>
       <c r="S3">
-        <v>0.4</v>
+        <v>0.007092198581560284</v>
       </c>
       <c r="T3">
-        <v>0.1333333333333333</v>
+        <v>0.03333333333333333</v>
       </c>
       <c r="U3">
-        <v>0.2</v>
+        <v>0.01169590643274854</v>
       </c>
     </row>
     <row r="4" spans="1:21">
@@ -667,13 +667,13 @@
         <v>22</v>
       </c>
       <c r="C4">
-        <v>38.5</v>
+        <v>46.67</v>
       </c>
       <c r="D4">
-        <v>9.800000000000001</v>
+        <v>13.73</v>
       </c>
       <c r="E4">
-        <v>15.6</v>
+        <v>21.21</v>
       </c>
       <c r="F4">
         <v>0</v>
@@ -688,40 +688,40 @@
         <v>28</v>
       </c>
       <c r="J4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="K4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="L4">
         <v>0</v>
       </c>
       <c r="M4">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="N4">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="O4">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="P4">
-        <v>38.5</v>
+        <v>46.67</v>
       </c>
       <c r="Q4">
-        <v>9.800000000000001</v>
+        <v>13.73</v>
       </c>
       <c r="R4">
-        <v>15.6</v>
+        <v>21.21</v>
       </c>
       <c r="S4">
-        <v>0.3846153846153846</v>
+        <v>0.4</v>
       </c>
       <c r="T4">
-        <v>0.1666666666666667</v>
+        <v>0.2</v>
       </c>
       <c r="U4">
-        <v>0.2325581395348837</v>
+        <v>0.2666666666666667</v>
       </c>
     </row>
     <row r="5" spans="1:21">
@@ -732,13 +732,13 @@
         <v>23</v>
       </c>
       <c r="C5">
-        <v>1.4</v>
+        <v>0.51</v>
       </c>
       <c r="D5">
-        <v>3.9</v>
+        <v>1.96</v>
       </c>
       <c r="E5">
-        <v>2.1</v>
+        <v>0.8099999999999999</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -753,40 +753,40 @@
         <v>28</v>
       </c>
       <c r="J5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K5">
-        <v>141</v>
+        <v>195</v>
       </c>
       <c r="L5">
         <v>0</v>
       </c>
       <c r="M5">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="N5">
-        <v>141</v>
+        <v>195</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="P5">
-        <v>1.4</v>
+        <v>0.51</v>
       </c>
       <c r="Q5">
-        <v>3.9</v>
+        <v>1.96</v>
       </c>
       <c r="R5">
-        <v>2.1</v>
+        <v>0.8099999999999999</v>
       </c>
       <c r="S5">
-        <v>0.007092198581560284</v>
+        <v>0.005128205128205128</v>
       </c>
       <c r="T5">
         <v>0.03333333333333333</v>
       </c>
       <c r="U5">
-        <v>0.01169590643274854</v>
+        <v>0.008888888888888889</v>
       </c>
     </row>
     <row r="6" spans="1:21">
@@ -797,13 +797,13 @@
         <v>24</v>
       </c>
       <c r="C6">
-        <v>5</v>
+        <v>13.95</v>
       </c>
       <c r="D6">
-        <v>9.800000000000001</v>
+        <v>11.76</v>
       </c>
       <c r="E6">
-        <v>6.600000000000001</v>
+        <v>12.77</v>
       </c>
       <c r="F6">
         <v>0</v>
@@ -818,40 +818,40 @@
         <v>28</v>
       </c>
       <c r="J6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K6">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="L6">
         <v>0</v>
       </c>
       <c r="M6">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="N6">
-        <v>100</v>
+        <v>43</v>
       </c>
       <c r="O6">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="P6">
-        <v>5</v>
+        <v>13.95</v>
       </c>
       <c r="Q6">
-        <v>9.800000000000001</v>
+        <v>11.76</v>
       </c>
       <c r="R6">
-        <v>6.600000000000001</v>
+        <v>12.77</v>
       </c>
       <c r="S6">
-        <v>0.03</v>
+        <v>0.09302325581395349</v>
       </c>
       <c r="T6">
-        <v>0.1</v>
+        <v>0.1333333333333333</v>
       </c>
       <c r="U6">
-        <v>0.04615384615384615</v>
+        <v>0.1095890410958904</v>
       </c>
     </row>
     <row r="7" spans="1:21">
@@ -862,13 +862,13 @@
         <v>25</v>
       </c>
       <c r="C7">
-        <v>14</v>
+        <v>38.46</v>
       </c>
       <c r="D7">
-        <v>11.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E7">
-        <v>12.8</v>
+        <v>15.62</v>
       </c>
       <c r="F7">
         <v>0</v>
@@ -883,40 +883,40 @@
         <v>28</v>
       </c>
       <c r="J7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="K7">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="L7">
         <v>0</v>
       </c>
       <c r="M7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="N7">
-        <v>43</v>
+        <v>13</v>
       </c>
       <c r="O7">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="P7">
-        <v>14</v>
+        <v>38.46</v>
       </c>
       <c r="Q7">
-        <v>11.8</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="R7">
-        <v>12.8</v>
+        <v>15.62</v>
       </c>
       <c r="S7">
-        <v>0.09302325581395349</v>
+        <v>0.3846153846153846</v>
       </c>
       <c r="T7">
-        <v>0.1333333333333333</v>
+        <v>0.1666666666666667</v>
       </c>
       <c r="U7">
-        <v>0.1095890410958904</v>
+        <v>0.2325581395348837</v>
       </c>
     </row>
     <row r="8" spans="1:21">
@@ -927,13 +927,13 @@
         <v>26</v>
       </c>
       <c r="C8">
-        <v>46.7</v>
+        <v>5</v>
       </c>
       <c r="D8">
-        <v>13.7</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="E8">
-        <v>21.2</v>
+        <v>6.619999999999999</v>
       </c>
       <c r="F8">
         <v>0</v>
@@ -948,40 +948,40 @@
         <v>28</v>
       </c>
       <c r="J8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="K8">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="L8">
         <v>0</v>
       </c>
       <c r="M8">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="N8">
-        <v>15</v>
+        <v>100</v>
       </c>
       <c r="O8">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="P8">
-        <v>46.7</v>
+        <v>5</v>
       </c>
       <c r="Q8">
-        <v>13.7</v>
+        <v>9.800000000000001</v>
       </c>
       <c r="R8">
-        <v>21.2</v>
+        <v>6.619999999999999</v>
       </c>
       <c r="S8">
-        <v>0.4</v>
+        <v>0.03</v>
       </c>
       <c r="T8">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="U8">
-        <v>0.2666666666666667</v>
+        <v>0.04615384615384615</v>
       </c>
     </row>
     <row r="9" spans="1:21">
@@ -1025,13 +1025,13 @@
         <v>15</v>
       </c>
       <c r="P9">
-        <v>4.399999999999999</v>
+        <v>4.43</v>
       </c>
       <c r="Q9">
-        <v>43.1</v>
+        <v>43.14</v>
       </c>
       <c r="R9">
-        <v>8</v>
+        <v>8.029999999999999</v>
       </c>
       <c r="S9">
         <v>0.03018108651911469</v>

</xml_diff>